<commit_message>
Updated availability status to Out Of Stock in excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resource/testdata/OpenCartTestData.xlsx
+++ b/src/test/resource/testdata/OpenCartTestData.xlsx
@@ -1,14 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shani\eclipse-workspaceNaveenSessions\Aug2023POMSeries\src\test\resource\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8603EF76-57A3-41BE-948F-5C1A04B6B43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{1BEA11C2-14D1-44BA-A3C6-30F91C3CD8C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{9C2BCF35-CD0A-4A29-9AD5-136CF87789CE}"/>
   </bookViews>
@@ -18,7 +13,8 @@
     <sheet name="login" sheetId="3" r:id="rId3"/>
     <sheet name="productInfoData" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
   <si>
     <t>Rahul</t>
   </si>
@@ -211,6 +207,9 @@
   </si>
   <si>
     <t>700</t>
+  </si>
+  <si>
+    <t>Out Of Stock</t>
   </si>
 </sst>
 </file>
@@ -949,7 +948,7 @@
         <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Updated excel data for checking auto trigger from jenkins
</commit_message>
<xml_diff>
--- a/src/test/resource/testdata/OpenCartTestData.xlsx
+++ b/src/test/resource/testdata/OpenCartTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{1BEA11C2-14D1-44BA-A3C6-30F91C3CD8C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0279B59B-8277-4365-8418-F04B8C7325C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{9C2BCF35-CD0A-4A29-9AD5-136CF87789CE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{9C2BCF35-CD0A-4A29-9AD5-136CF87789CE}"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="1" r:id="rId1"/>
@@ -14,19 +14,10 @@
     <sheet name="productInfoData" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:K12"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -778,7 +769,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F3BBE2F-5C75-4203-A5FD-739870BBDD09}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -856,7 +849,7 @@
         <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -871,7 +864,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090243F3-6803-4661-B99B-94EA14C2E755}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
Updated testngregression file and excel data with space to test auto trigger
</commit_message>
<xml_diff>
--- a/src/test/resource/testdata/OpenCartTestData.xlsx
+++ b/src/test/resource/testdata/OpenCartTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0279B59B-8277-4365-8418-F04B8C7325C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2F854635-01ED-4CB5-9941-D2DEB9887499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{9C2BCF35-CD0A-4A29-9AD5-136CF87789CE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{9C2BCF35-CD0A-4A29-9AD5-136CF87789CE}"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="productInfoData" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K12"/>
+  <oleSize ref="A1:L12"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -769,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F3BBE2F-5C75-4203-A5FD-739870BBDD09}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -849,7 +849,7 @@
         <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -864,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090243F3-6803-4661-B99B-94EA14C2E755}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>